<commit_message>
update idea of interface
</commit_message>
<xml_diff>
--- a/FactoringCapインターフェース.xlsx
+++ b/FactoringCapインターフェース.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="800" windowWidth="19220" windowHeight="13760" tabRatio="500"/>
+    <workbookView xWindow="9920" yWindow="3500" windowWidth="17440" windowHeight="13160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>FactoringCap</t>
     <phoneticPr fontId="1"/>
@@ -210,6 +211,34 @@
     </rPh>
     <rPh sb="28" eb="30">
       <t>ブブン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>caplet volカーブ構築</t>
+    <rPh sb="13" eb="15">
+      <t>コウチク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cap vol計算</t>
+    <rPh sb="7" eb="9">
+      <t>ケイサン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cap volからcaplet volへ分解</t>
+    <rPh sb="20" eb="22">
+      <t>ブンカイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>caplet PVを計算</t>
+    <rPh sb="10" eb="12">
+      <t>ケイサン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -590,7 +619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A10" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -695,4 +724,43 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="2:5">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>